<commit_message>
feat: Add orderLink field to material lifecycle rules
Materials in 'ordered' status now ask for order link (e.g., Amazon URL)
after the expected delivery date is set. The link helps track purchases.

Changes:
- Added orderLink question in getMaterialQuestion() for ordered materials
- Updated completeness check to include orderLink for ordered status
- Added Order Link column to Materials export sheet
- Users can answer 'N/A' if no link is applicable

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/projects/kitchen-remodel/Kitchen-Remodel-Tracker.xlsx
+++ b/projects/kitchen-remodel/Kitchen-Remodel-Tracker.xlsx
@@ -15,9 +15,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">'Schedule'!A1:K75</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">'By Assignee'!A1:I103</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">'Tasks'!A1:M75</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4">'Materials'!A1:K16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4">'Materials'!A1:L16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Vendors'!A1:G15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6">'Open Questions'!A1:K24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6">'Open Questions'!A1:K27</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -10005,7 +10005,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10013,14 +10013,15 @@
     <col min="1" max="1" width="30.83203125" customWidth="1"/>
     <col min="2" max="2" width="35.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" customWidth="1"/>
     <col min="5" max="5" width="30.83203125" customWidth="1"/>
     <col min="6" max="6" width="35.83203125" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="25.83203125" customWidth="1"/>
-    <col min="10" max="10" width="40.83203125" customWidth="1"/>
+    <col min="9" max="9" width="40.83203125" customWidth="1"/>
+    <col min="10" max="10" width="25.83203125" customWidth="1"/>
     <col min="11" max="11" width="40.83203125" customWidth="1"/>
+    <col min="12" max="12" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -10049,12 +10050,15 @@
         <v>Expected Date</v>
       </c>
       <c r="I1" s="8" t="str">
+        <v>Order Link</v>
+      </c>
+      <c r="J1" s="8" t="str">
         <v>Detail</v>
       </c>
-      <c r="J1" s="8" t="str">
+      <c r="K1" s="8" t="str">
         <v>Notes</v>
       </c>
-      <c r="K1" s="8" t="str">
+      <c r="L1" s="8" t="str">
         <v>Comments</v>
       </c>
     </row>
@@ -10092,6 +10096,9 @@
       <c r="K2" s="19" t="str">
         <v/>
       </c>
+      <c r="L2" s="19" t="str">
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="12" t="str">
@@ -10122,9 +10129,12 @@
         <v/>
       </c>
       <c r="J3" s="12" t="str">
+        <v/>
+      </c>
+      <c r="K3" s="12" t="str">
         <v>In garage.</v>
       </c>
-      <c r="K3" s="12" t="str">
+      <c r="L3" s="12" t="str">
         <v/>
       </c>
     </row>
@@ -10157,9 +10167,12 @@
         <v/>
       </c>
       <c r="J4" s="19" t="str">
+        <v/>
+      </c>
+      <c r="K4" s="19" t="str">
         <v>In garage.</v>
       </c>
-      <c r="K4" s="19" t="str">
+      <c r="L4" s="19" t="str">
         <v/>
       </c>
     </row>
@@ -10192,9 +10205,12 @@
         <v/>
       </c>
       <c r="J5" s="12" t="str">
+        <v/>
+      </c>
+      <c r="K5" s="12" t="str">
         <v>Existing 32" door.</v>
       </c>
-      <c r="K5" s="12" t="str">
+      <c r="L5" s="12" t="str">
         <v/>
       </c>
     </row>
@@ -10209,7 +10225,7 @@
         <v>ordered</v>
       </c>
       <c r="D6" s="19" t="str">
-        <v>✅ Complete</v>
+        <v>⚠️ Missing: orderLink</v>
       </c>
       <c r="E6" s="19" t="str">
         <v>install-doors</v>
@@ -10230,6 +10246,9 @@
         <v/>
       </c>
       <c r="K6" s="19" t="str">
+        <v/>
+      </c>
+      <c r="L6" s="19" t="str">
         <v/>
       </c>
     </row>
@@ -10244,7 +10263,7 @@
         <v>ordered</v>
       </c>
       <c r="D7" s="12" t="str">
-        <v>⚠️ Missing: expectedDate</v>
+        <v>⚠️ Missing: expectedDate, orderLink</v>
       </c>
       <c r="E7" s="12" t="str">
         <v>install-doors</v>
@@ -10259,12 +10278,15 @@
         <v/>
       </c>
       <c r="I7" s="12" t="str">
+        <v/>
+      </c>
+      <c r="J7" s="12" t="str">
         <v>4" Antique Bronze</v>
       </c>
-      <c r="J7" s="12" t="str">
-        <v/>
-      </c>
       <c r="K7" s="12" t="str">
+        <v/>
+      </c>
+      <c r="L7" s="12" t="str">
         <v/>
       </c>
     </row>
@@ -10279,7 +10301,7 @@
         <v>ordered</v>
       </c>
       <c r="D8" s="19" t="str">
-        <v>⚠️ Missing: expectedDate</v>
+        <v>⚠️ Missing: expectedDate, orderLink</v>
       </c>
       <c r="E8" s="19" t="str">
         <v>install-doors</v>
@@ -10294,12 +10316,15 @@
         <v/>
       </c>
       <c r="I8" s="19" t="str">
+        <v/>
+      </c>
+      <c r="J8" s="19" t="str">
         <v>Antique Bronze</v>
       </c>
-      <c r="J8" s="19" t="str">
-        <v/>
-      </c>
       <c r="K8" s="19" t="str">
+        <v/>
+      </c>
+      <c r="L8" s="19" t="str">
         <v/>
       </c>
     </row>
@@ -10329,12 +10354,15 @@
         <v/>
       </c>
       <c r="I9" s="12" t="str">
+        <v/>
+      </c>
+      <c r="J9" s="12" t="str">
         <v>Antique Bronze</v>
       </c>
-      <c r="J9" s="12" t="str">
-        <v/>
-      </c>
       <c r="K9" s="12" t="str">
+        <v/>
+      </c>
+      <c r="L9" s="12" t="str">
         <v/>
       </c>
     </row>
@@ -10349,7 +10377,7 @@
         <v>ordered</v>
       </c>
       <c r="D10" s="19" t="str">
-        <v>⚠️ Missing: expectedDate</v>
+        <v>⚠️ Missing: expectedDate, orderLink</v>
       </c>
       <c r="E10" s="19" t="str">
         <v>install-doors</v>
@@ -10364,12 +10392,15 @@
         <v/>
       </c>
       <c r="I10" s="19" t="str">
+        <v/>
+      </c>
+      <c r="J10" s="19" t="str">
         <v>Antique Bronze</v>
       </c>
-      <c r="J10" s="19" t="str">
-        <v/>
-      </c>
       <c r="K10" s="19" t="str">
+        <v/>
+      </c>
+      <c r="L10" s="19" t="str">
         <v/>
       </c>
     </row>
@@ -10407,6 +10438,9 @@
       <c r="K11" s="12" t="str">
         <v/>
       </c>
+      <c r="L11" s="12" t="str">
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="19" t="str">
@@ -10437,9 +10471,12 @@
         <v/>
       </c>
       <c r="J12" s="19" t="str">
+        <v/>
+      </c>
+      <c r="K12" s="19" t="str">
         <v>Get count.</v>
       </c>
-      <c r="K12" s="19" t="str">
+      <c r="L12" s="19" t="str">
         <v/>
       </c>
     </row>
@@ -10477,6 +10514,9 @@
       <c r="K13" s="12" t="str">
         <v/>
       </c>
+      <c r="L13" s="12" t="str">
+        <v/>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="19" t="str">
@@ -10489,7 +10529,7 @@
         <v>ordered</v>
       </c>
       <c r="D14" s="19" t="str">
-        <v>✅ Complete</v>
+        <v>⚠️ Missing: orderLink</v>
       </c>
       <c r="E14" s="19" t="str">
         <v>misc-equipment-install</v>
@@ -10510,6 +10550,9 @@
         <v/>
       </c>
       <c r="K14" s="19" t="str">
+        <v/>
+      </c>
+      <c r="L14" s="19" t="str">
         <v/>
       </c>
     </row>
@@ -10524,7 +10567,7 @@
         <v>ordered</v>
       </c>
       <c r="D15" s="12" t="str">
-        <v>✅ Complete</v>
+        <v>⚠️ Missing: orderLink</v>
       </c>
       <c r="E15" s="12" t="str">
         <v>upper-cabinet-install</v>
@@ -10545,6 +10588,9 @@
         <v/>
       </c>
       <c r="K15" s="12" t="str">
+        <v/>
+      </c>
+      <c r="L15" s="12" t="str">
         <v/>
       </c>
     </row>
@@ -10559,7 +10605,7 @@
         <v>ordered</v>
       </c>
       <c r="D16" s="19" t="str">
-        <v>⚠️ Missing: expectedDate</v>
+        <v>⚠️ Missing: expectedDate, orderLink</v>
       </c>
       <c r="E16" s="19" t="str">
         <v>upper-cabinet-install</v>
@@ -10582,12 +10628,15 @@
       <c r="K16" s="19" t="str">
         <v/>
       </c>
+      <c r="L16" s="19" t="str">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <autoFilter ref="A1:K16"/>
+  <autoFilter ref="A1:L16"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L16"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -10964,7 +11013,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11822,10 +11871,115 @@
         <v/>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" s="12" t="str">
+        <v>sq-free-text-hinges-main-kitchen-door-orderLink</v>
+      </c>
+      <c r="B25" s="12" t="str">
+        <v>Free Text</v>
+      </c>
+      <c r="C25" s="12" t="str">
+        <v>2026-01-21</v>
+      </c>
+      <c r="D25" s="12" t="str">
+        <v>What is the order link for "Hinges (Main Kitchen Door)"? (e.g., Amazon order URL, or 'N/A' if not applicable)</v>
+      </c>
+      <c r="E25" s="12" t="str">
+        <v>Tonia</v>
+      </c>
+      <c r="F25" s="12" t="str">
+        <v>install-doors</v>
+      </c>
+      <c r="G25" s="12" t="str">
+        <v>hinges-main-kitchen-door</v>
+      </c>
+      <c r="H25" s="12" t="str">
+        <v/>
+      </c>
+      <c r="I25" s="12" t="str">
+        <v/>
+      </c>
+      <c r="J25" s="12" t="str">
+        <v>Open</v>
+      </c>
+      <c r="K25" s="12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="20" t="str">
+        <v>sq-free-text-retractable-extension-cord-orderLink</v>
+      </c>
+      <c r="B26" s="20" t="str">
+        <v>Free Text</v>
+      </c>
+      <c r="C26" s="20" t="str">
+        <v>2026-01-21</v>
+      </c>
+      <c r="D26" s="20" t="str">
+        <v>What is the order link for "Retractable Extension Cord"? (e.g., Amazon order URL, or 'N/A' if not applicable)</v>
+      </c>
+      <c r="E26" s="20" t="str">
+        <v>Tonia</v>
+      </c>
+      <c r="F26" s="20" t="str">
+        <v>misc-equipment-install</v>
+      </c>
+      <c r="G26" s="20" t="str">
+        <v>retractable-extension-cord</v>
+      </c>
+      <c r="H26" s="20" t="str">
+        <v/>
+      </c>
+      <c r="I26" s="20" t="str">
+        <v/>
+      </c>
+      <c r="J26" s="20" t="str">
+        <v>Open</v>
+      </c>
+      <c r="K26" s="20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="12" t="str">
+        <v>sq-free-text-upper-cabinets-orderLink</v>
+      </c>
+      <c r="B27" s="12" t="str">
+        <v>Free Text</v>
+      </c>
+      <c r="C27" s="12" t="str">
+        <v>2026-01-21</v>
+      </c>
+      <c r="D27" s="12" t="str">
+        <v>What is the order link for "Upper Cabinets"? (e.g., Amazon order URL, or 'N/A' if not applicable)</v>
+      </c>
+      <c r="E27" s="12" t="str">
+        <v>Tonia</v>
+      </c>
+      <c r="F27" s="12" t="str">
+        <v>upper-cabinet-install</v>
+      </c>
+      <c r="G27" s="12" t="str">
+        <v>upper-cabinets</v>
+      </c>
+      <c r="H27" s="12" t="str">
+        <v/>
+      </c>
+      <c r="I27" s="12" t="str">
+        <v/>
+      </c>
+      <c r="J27" s="12" t="str">
+        <v>Open</v>
+      </c>
+      <c r="K27" s="12" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K24"/>
+  <autoFilter ref="A1:K27"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K24"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Combined delivery date + order link question for ordered materials
When a material is marked as ordered and is missing BOTH expectedDate
and orderLink, we now ask a single combined question instead of two
separate ones to minimize question count.

Example: "For X: What is the expected delivery date and order link?
(e.g., '2026-01-25, https://amazon.com/...' or '2026-01-25, N/A')"

Changes:
- Added parseDateAndLink() to extract date and URL from combined response
- Updated getMaterialQuestion() to use combined question when both missing
- Improved materialQuestionExists() to detect overlapping field coverage
- Cleaned up duplicate questions from previous separate approach

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/projects/kitchen-remodel/Kitchen-Remodel-Tracker.xlsx
+++ b/projects/kitchen-remodel/Kitchen-Remodel-Tracker.xlsx
@@ -11698,25 +11698,25 @@
     </row>
     <row r="20">
       <c r="A20" s="20" t="str">
-        <v>sq-date-hinges-back-door-expectedDate</v>
+        <v>sq-free-text-receptacle-light-switch-covers-quantity-detail</v>
       </c>
       <c r="B20" s="20" t="str">
-        <v>Date</v>
+        <v>Free Text</v>
       </c>
       <c r="C20" s="20" t="str">
         <v>2026-01-21</v>
       </c>
       <c r="D20" s="20" t="str">
-        <v>When is "Hinges (Back Door)" expected to arrive?</v>
+        <v>How many "Receptacle and Light Switch Covers" are needed, and what are the specifications? (Answer 'N/A' for specs if not applicable)</v>
       </c>
       <c r="E20" s="20" t="str">
         <v>Tonia</v>
       </c>
       <c r="F20" s="20" t="str">
-        <v>install-doors</v>
+        <v>finish-electrical</v>
       </c>
       <c r="G20" s="20" t="str">
-        <v>hinges-back-door</v>
+        <v>receptacle-light-switch-covers</v>
       </c>
       <c r="H20" s="20" t="str">
         <v/>
@@ -11733,16 +11733,16 @@
     </row>
     <row r="21">
       <c r="A21" s="12" t="str">
-        <v>sq-date-doorknob-back-door-expectedDate</v>
+        <v>sq-free-text-hinges-main-kitchen-door-orderLink</v>
       </c>
       <c r="B21" s="12" t="str">
-        <v>Date</v>
+        <v>Free Text</v>
       </c>
       <c r="C21" s="12" t="str">
         <v>2026-01-21</v>
       </c>
       <c r="D21" s="12" t="str">
-        <v>When is "Doorknob (Back Door)" expected to arrive?</v>
+        <v>What is the order link for "Hinges (Main Kitchen Door)"? (e.g., Amazon order URL, or 'N/A' if not applicable)</v>
       </c>
       <c r="E21" s="12" t="str">
         <v>Tonia</v>
@@ -11751,7 +11751,7 @@
         <v>install-doors</v>
       </c>
       <c r="G21" s="12" t="str">
-        <v>doorknob-back-door</v>
+        <v>hinges-main-kitchen-door</v>
       </c>
       <c r="H21" s="12" t="str">
         <v/>
@@ -11768,25 +11768,25 @@
     </row>
     <row r="22">
       <c r="A22" s="20" t="str">
-        <v>sq-date-doorknob-hinges-hvac-expectedDate</v>
+        <v>sq-free-text-retractable-extension-cord-orderLink</v>
       </c>
       <c r="B22" s="20" t="str">
-        <v>Date</v>
+        <v>Free Text</v>
       </c>
       <c r="C22" s="20" t="str">
         <v>2026-01-21</v>
       </c>
       <c r="D22" s="20" t="str">
-        <v>When is "Doorknob &amp; Hinges (HVAC)" expected to arrive?</v>
+        <v>What is the order link for "Retractable Extension Cord"? (e.g., Amazon order URL, or 'N/A' if not applicable)</v>
       </c>
       <c r="E22" s="20" t="str">
         <v>Tonia</v>
       </c>
       <c r="F22" s="20" t="str">
-        <v>install-doors</v>
+        <v>misc-equipment-install</v>
       </c>
       <c r="G22" s="20" t="str">
-        <v>doorknob-hinges-hvac</v>
+        <v>retractable-extension-cord</v>
       </c>
       <c r="H22" s="20" t="str">
         <v/>
@@ -11803,7 +11803,7 @@
     </row>
     <row r="23">
       <c r="A23" s="12" t="str">
-        <v>sq-free-text-receptacle-light-switch-covers-quantity-detail</v>
+        <v>sq-free-text-upper-cabinets-orderLink</v>
       </c>
       <c r="B23" s="12" t="str">
         <v>Free Text</v>
@@ -11812,16 +11812,16 @@
         <v>2026-01-21</v>
       </c>
       <c r="D23" s="12" t="str">
-        <v>How many "Receptacle and Light Switch Covers" are needed, and what are the specifications? (Answer 'N/A' for specs if not applicable)</v>
+        <v>What is the order link for "Upper Cabinets"? (e.g., Amazon order URL, or 'N/A' if not applicable)</v>
       </c>
       <c r="E23" s="12" t="str">
         <v>Tonia</v>
       </c>
       <c r="F23" s="12" t="str">
-        <v>finish-electrical</v>
+        <v>upper-cabinet-install</v>
       </c>
       <c r="G23" s="12" t="str">
-        <v>receptacle-light-switch-covers</v>
+        <v>upper-cabinets</v>
       </c>
       <c r="H23" s="12" t="str">
         <v/>
@@ -11838,25 +11838,25 @@
     </row>
     <row r="24">
       <c r="A24" s="20" t="str">
-        <v>sq-date-upper-cabinet-handles-expectedDate</v>
+        <v>sq-free-text-hinges-back-door-expectedDate-orderLink</v>
       </c>
       <c r="B24" s="20" t="str">
-        <v>Date</v>
+        <v>Free Text</v>
       </c>
       <c r="C24" s="20" t="str">
         <v>2026-01-21</v>
       </c>
       <c r="D24" s="20" t="str">
-        <v>When is "Upper Cabinet Handles" expected to arrive?</v>
+        <v>For "Hinges (Back Door)": What is the expected delivery date and order link? (e.g., "2026-01-25, https://amazon.com/..." or "2026-01-25, N/A")</v>
       </c>
       <c r="E24" s="20" t="str">
         <v>Tonia</v>
       </c>
       <c r="F24" s="20" t="str">
-        <v>upper-cabinet-install</v>
+        <v>install-doors</v>
       </c>
       <c r="G24" s="20" t="str">
-        <v>upper-cabinet-handles</v>
+        <v>hinges-back-door</v>
       </c>
       <c r="H24" s="20" t="str">
         <v/>
@@ -11873,7 +11873,7 @@
     </row>
     <row r="25">
       <c r="A25" s="12" t="str">
-        <v>sq-free-text-hinges-main-kitchen-door-orderLink</v>
+        <v>sq-free-text-doorknob-back-door-expectedDate-orderLink</v>
       </c>
       <c r="B25" s="12" t="str">
         <v>Free Text</v>
@@ -11882,7 +11882,7 @@
         <v>2026-01-21</v>
       </c>
       <c r="D25" s="12" t="str">
-        <v>What is the order link for "Hinges (Main Kitchen Door)"? (e.g., Amazon order URL, or 'N/A' if not applicable)</v>
+        <v>For "Doorknob (Back Door)": What is the expected delivery date and order link? (e.g., "2026-01-25, https://amazon.com/..." or "2026-01-25, N/A")</v>
       </c>
       <c r="E25" s="12" t="str">
         <v>Tonia</v>
@@ -11891,7 +11891,7 @@
         <v>install-doors</v>
       </c>
       <c r="G25" s="12" t="str">
-        <v>hinges-main-kitchen-door</v>
+        <v>doorknob-back-door</v>
       </c>
       <c r="H25" s="12" t="str">
         <v/>
@@ -11908,7 +11908,7 @@
     </row>
     <row r="26">
       <c r="A26" s="20" t="str">
-        <v>sq-free-text-retractable-extension-cord-orderLink</v>
+        <v>sq-free-text-doorknob-hinges-hvac-expectedDate-orderLink</v>
       </c>
       <c r="B26" s="20" t="str">
         <v>Free Text</v>
@@ -11917,16 +11917,16 @@
         <v>2026-01-21</v>
       </c>
       <c r="D26" s="20" t="str">
-        <v>What is the order link for "Retractable Extension Cord"? (e.g., Amazon order URL, or 'N/A' if not applicable)</v>
+        <v>For "Doorknob &amp; Hinges (HVAC)": What is the expected delivery date and order link? (e.g., "2026-01-25, https://amazon.com/..." or "2026-01-25, N/A")</v>
       </c>
       <c r="E26" s="20" t="str">
         <v>Tonia</v>
       </c>
       <c r="F26" s="20" t="str">
-        <v>misc-equipment-install</v>
+        <v>install-doors</v>
       </c>
       <c r="G26" s="20" t="str">
-        <v>retractable-extension-cord</v>
+        <v>doorknob-hinges-hvac</v>
       </c>
       <c r="H26" s="20" t="str">
         <v/>
@@ -11943,7 +11943,7 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="str">
-        <v>sq-free-text-upper-cabinets-orderLink</v>
+        <v>sq-free-text-upper-cabinet-handles-expectedDate-orderLink</v>
       </c>
       <c r="B27" s="12" t="str">
         <v>Free Text</v>
@@ -11952,7 +11952,7 @@
         <v>2026-01-21</v>
       </c>
       <c r="D27" s="12" t="str">
-        <v>What is the order link for "Upper Cabinets"? (e.g., Amazon order URL, or 'N/A' if not applicable)</v>
+        <v>For "Upper Cabinet Handles": What is the expected delivery date and order link? (e.g., "2026-01-25, https://amazon.com/..." or "2026-01-25, N/A")</v>
       </c>
       <c r="E27" s="12" t="str">
         <v>Tonia</v>
@@ -11961,7 +11961,7 @@
         <v>upper-cabinet-install</v>
       </c>
       <c r="G27" s="12" t="str">
-        <v>upper-cabinets</v>
+        <v>upper-cabinet-handles</v>
       </c>
       <c r="H27" s="12" t="str">
         <v/>

</xml_diff>

<commit_message>
feat: Add vendor-provided material status
Materials provided by vendors as part of their work scope (like HVAC
registers from Joclar & Fields) don't need order tracking. This status
skips expectedDate and orderLink validation while still requiring
quantity and specs.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/projects/kitchen-remodel/Kitchen-Remodel-Tracker.xlsx
+++ b/projects/kitchen-remodel/Kitchen-Remodel-Tracker.xlsx
@@ -9,15 +9,15 @@
     <sheet name="Tasks" sheetId="4" r:id="rId4"/>
     <sheet name="Materials" sheetId="5" r:id="rId5"/>
     <sheet name="Vendors" sheetId="6" r:id="rId6"/>
-    <sheet name="Open Questions" sheetId="7" r:id="rId7"/>
+    <sheet name="Issues" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'Schedule'!A1:K79</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'By Assignee'!A1:I109</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3">'Tasks'!A1:M81</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4">'Materials'!A1:L16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'Schedule'!A1:K80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'By Assignee'!A1:I110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3">'Tasks'!A1:M82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4">'Materials'!A1:L18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Vendors'!A1:G15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6">'Open Questions'!A1:L83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6">'Issues'!A1:L83</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -942,7 +942,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A74"/>
+  <dimension ref="A1:A80"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -987,7 +987,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>📋 OPEN QUESTIONS</v>
+        <v>📋 ISSUES</v>
       </c>
     </row>
     <row r="9">
@@ -997,7 +997,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="str">
-        <v>Questions that need your input. Find your name in the Assignee column</v>
+        <v>Issues that need your input. Find your name in the Assignee column</v>
       </c>
     </row>
     <row r="11">
@@ -1017,7 +1017,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="str">
-        <v>question disappears from this list.</v>
+        <v>issue disappears from this list.</v>
       </c>
     </row>
     <row r="15">
@@ -1027,57 +1027,57 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="str">
-        <v xml:space="preserve">  • Yellow rows = Waiting for your answer</v>
+        <v>Row colors indicate action needed:</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="str">
-        <v/>
+        <v xml:space="preserve">  • Blue = Assign (Who should do this?)</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="str">
-        <v>━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━</v>
+        <v xml:space="preserve">  • Orange = Schedule (When should this happen?)</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="str">
-        <v/>
+        <v xml:space="preserve">  • Green = Order (Ready to purchase?)</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>📅 SCHEDULE</v>
+        <v xml:space="preserve">  • Yellow = Specify (Need specs/quantity)</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="str">
-        <v/>
+        <v xml:space="preserve">  • Purple = Track (Need delivery info)</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="str">
-        <v>Shows tasks in the order they can be done - what needs to finish</v>
+        <v xml:space="preserve">  • White = Decide (Decision needed)</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="str">
-        <v>before something else can start.</v>
+        <v/>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="str">
-        <v/>
+        <v>━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="str">
-        <v>Use this to see what's next and what's blocking progress.</v>
+        <v/>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="str">
-        <v>Check the Issues column (in red) for problems that need attention.</v>
+        <v>📅 SCHEDULE</v>
       </c>
     </row>
     <row r="27">
@@ -1087,250 +1087,280 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="str">
-        <v>━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━</v>
+        <v>Shows tasks in the order they can be done - what needs to finish</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="str">
-        <v/>
+        <v>before something else can start.</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>👤 BY ASSIGNEE</v>
+        <v/>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="str">
-        <v/>
+        <v>Use this to see what's next and what's blocking progress.</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="str">
-        <v>Tasks grouped by who's responsible.</v>
+        <v>Check the Issues column (in red) for problems that need attention.</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="str">
-        <v>See your workload at a glance, or check what others are working on.</v>
+        <v/>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="str">
-        <v/>
+        <v>━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="str">
-        <v>━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━</v>
+        <v/>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="str">
-        <v/>
+        <v>👤 BY ASSIGNEE</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="4" t="str">
-        <v>📝 TASKS</v>
+        <v/>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="str">
-        <v/>
+        <v>Tasks grouped by who's responsible.</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="str">
-        <v>The master list of all tasks with full details - dates, dependencies,</v>
+        <v>See your workload at a glance, or check what others are working on.</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="str">
-        <v>notes, and materials needed.</v>
+        <v/>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="str">
-        <v/>
+        <v>━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="str">
-        <v>Look here when you need the complete picture on any task.</v>
+        <v/>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="str">
-        <v/>
+        <v>📝 TASKS</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="str">
-        <v>Ready column shows if we have all needed info:</v>
+        <v/>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="str">
-        <v xml:space="preserve">  • ✅ Yes = Has dates and assignee</v>
+        <v>The master list of all tasks with full details - dates, dependencies,</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="str">
-        <v xml:space="preserve">  • ⚠️ Missing: dates = Needs start/end dates</v>
+        <v>notes, and materials needed.</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="str">
-        <v xml:space="preserve">  • ⚠️ Missing: assignee = Needs someone assigned</v>
+        <v/>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="str">
-        <v/>
+        <v>Look here when you need the complete picture on any task.</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="str">
-        <v>━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━</v>
+        <v/>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="4" t="str">
-        <v/>
+        <v>Ready column shows if we have all needed info:</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="str">
-        <v>📦 MATERIALS</v>
+        <v xml:space="preserve">  • ✅ Yes = Has dates and assignee</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="str">
-        <v/>
+        <v xml:space="preserve">  • ⚠️ Missing: dates = Needs start/end dates</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="str">
-        <v>All materials needed for the project - what's on-hand, what's ordered,</v>
+        <v xml:space="preserve">  • ⚠️ Missing: assignee = Needs someone assigned</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="str">
-        <v>what still needs to be purchased.</v>
+        <v/>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="str">
-        <v/>
+        <v>━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="str">
-        <v>Check expected delivery dates and order links here.</v>
+        <v/>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="str">
-        <v/>
+        <v>📦 MATERIALS</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="str">
-        <v>Ready column shows if we have all needed info for that status:</v>
+        <v/>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="str">
-        <v xml:space="preserve">  • ✅ Yes = Has everything needed</v>
+        <v>All materials needed for the project - what's on-hand, what's ordered,</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="str">
-        <v xml:space="preserve">  • ⚠️ Missing: specs = Needs specs/details</v>
+        <v>what still needs to be purchased.</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="str">
-        <v xml:space="preserve">  • ⚠️ Missing: quantity = Needs quantity</v>
+        <v/>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="str">
-        <v xml:space="preserve">  • ⚠️ Missing: expectedDate = Needs delivery date</v>
+        <v>Check expected delivery dates and order links here.</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="str">
-        <v xml:space="preserve">  • ⚠️ Missing: orderLink = Needs order link</v>
+        <v/>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="str">
-        <v/>
+        <v>Ready column shows if we have all needed info for that status:</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="str">
-        <v>━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━</v>
+        <v xml:space="preserve">  • ✅ Yes = Has everything needed</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="4" t="str">
-        <v/>
+        <v xml:space="preserve">  • ⚠️ Missing: specs = Needs specs/details</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="str">
-        <v>NOTES</v>
+        <v xml:space="preserve">  • ⚠️ Missing: quantity = Needs quantity</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="str">
-        <v/>
+        <v xml:space="preserve">  • ⚠️ Missing: expectedDate = Needs delivery date</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="str">
-        <v>• You can't break anything - other tabs are protected</v>
+        <v xml:space="preserve">  • ⚠️ Missing: orderLink = Needs order link</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="str">
-        <v>• After you answer, changes appear in the next update</v>
+        <v/>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="str">
-        <v>• View this on a computer - it's too complex for mobile</v>
+        <v>━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━━</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="str">
-        <v>• Questions? Contact Dave</v>
+        <v/>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="str">
-        <v/>
+        <v>NOTES</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="str">
+        <v>• You can't break anything - other tabs are protected</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="str">
+        <v>• After you answer, changes appear in the next update</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="str">
+        <v>• View this on a computer - it's too complex for mobile</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="str">
+        <v>• Questions? Contact Dave</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="str">
         <v>Last updated: Thursday, January 22, 2026</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A74"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A80"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4113,18 +4143,53 @@
         <v>No assignee</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" s="7">
+        <v>79</v>
+      </c>
+      <c r="B80" s="7" t="str">
+        <v>TASK</v>
+      </c>
+      <c r="C80" s="7" t="str">
+        <v>hvac-finish</v>
+      </c>
+      <c r="D80" s="7" t="str">
+        <v>Schedule HVAC Finish</v>
+      </c>
+      <c r="E80" s="7" t="str">
+        <v>needs-scheduled</v>
+      </c>
+      <c r="F80" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G80" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H80" s="7" t="str">
+        <v>2026-01-22</v>
+      </c>
+      <c r="I80" s="7" t="str">
+        <v>Joclar &amp; Fields</v>
+      </c>
+      <c r="J80" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K80" s="7" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <autoFilter ref="A1:K79"/>
+  <autoFilter ref="A1:K80"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K79"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K80"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6645,7 +6710,7 @@
     </row>
     <row r="87">
       <c r="A87" s="16" t="str">
-        <v>▶ Joclar &amp; Fields (1 items)</v>
+        <v>▶ Joclar &amp; Fields (2 items)</v>
       </c>
       <c r="B87" s="16" t="str">
         <v/>
@@ -6702,89 +6767,89 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="2" t="str">
-        <v/>
-      </c>
-      <c r="B89" s="2" t="str">
-        <v/>
-      </c>
-      <c r="C89" s="2" t="str">
-        <v/>
-      </c>
-      <c r="D89" s="2" t="str">
-        <v/>
-      </c>
-      <c r="E89" s="2" t="str">
-        <v/>
-      </c>
-      <c r="F89" s="2" t="str">
-        <v/>
-      </c>
-      <c r="G89" s="2" t="str">
-        <v/>
-      </c>
-      <c r="H89" s="2" t="str">
-        <v/>
-      </c>
-      <c r="I89" s="2" t="str">
+      <c r="A89" s="9" t="str">
+        <v/>
+      </c>
+      <c r="B89" s="9" t="str">
+        <v>hvac-finish</v>
+      </c>
+      <c r="C89" s="9" t="str">
+        <v>Schedule HVAC Finish</v>
+      </c>
+      <c r="D89" s="9" t="str">
+        <v>needs-scheduled</v>
+      </c>
+      <c r="E89" s="9" t="str">
+        <v/>
+      </c>
+      <c r="F89" s="9" t="str">
+        <v/>
+      </c>
+      <c r="G89" s="9" t="str">
+        <v/>
+      </c>
+      <c r="H89" s="9" t="str">
+        <v/>
+      </c>
+      <c r="I89" s="9" t="str">
         <v/>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="16" t="str">
+      <c r="A90" s="2" t="str">
+        <v/>
+      </c>
+      <c r="B90" s="2" t="str">
+        <v/>
+      </c>
+      <c r="C90" s="2" t="str">
+        <v/>
+      </c>
+      <c r="D90" s="2" t="str">
+        <v/>
+      </c>
+      <c r="E90" s="2" t="str">
+        <v/>
+      </c>
+      <c r="F90" s="2" t="str">
+        <v/>
+      </c>
+      <c r="G90" s="2" t="str">
+        <v/>
+      </c>
+      <c r="H90" s="2" t="str">
+        <v/>
+      </c>
+      <c r="I90" s="2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="16" t="str">
         <v>▶ Sergio (2 items)</v>
       </c>
-      <c r="B90" s="16" t="str">
-        <v/>
-      </c>
-      <c r="C90" s="16" t="str">
-        <v/>
-      </c>
-      <c r="D90" s="16" t="str">
-        <v/>
-      </c>
-      <c r="E90" s="16" t="str">
-        <v/>
-      </c>
-      <c r="F90" s="16" t="str">
-        <v/>
-      </c>
-      <c r="G90" s="16" t="str">
-        <v/>
-      </c>
-      <c r="H90" s="16" t="str">
-        <v/>
-      </c>
-      <c r="I90" s="16" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="9" t="str">
-        <v/>
-      </c>
-      <c r="B91" s="9" t="str">
-        <v>siding</v>
-      </c>
-      <c r="C91" s="9" t="str">
-        <v>Siding</v>
-      </c>
-      <c r="D91" s="9" t="str">
-        <v>needs-scheduled</v>
-      </c>
-      <c r="E91" s="9" t="str">
-        <v/>
-      </c>
-      <c r="F91" s="9" t="str">
-        <v/>
-      </c>
-      <c r="G91" s="9" t="str">
-        <v>propane</v>
-      </c>
-      <c r="H91" s="9" t="str">
-        <v/>
-      </c>
-      <c r="I91" s="9" t="str">
+      <c r="B91" s="16" t="str">
+        <v/>
+      </c>
+      <c r="C91" s="16" t="str">
+        <v/>
+      </c>
+      <c r="D91" s="16" t="str">
+        <v/>
+      </c>
+      <c r="E91" s="16" t="str">
+        <v/>
+      </c>
+      <c r="F91" s="16" t="str">
+        <v/>
+      </c>
+      <c r="G91" s="16" t="str">
+        <v/>
+      </c>
+      <c r="H91" s="16" t="str">
+        <v/>
+      </c>
+      <c r="I91" s="16" t="str">
         <v/>
       </c>
     </row>
@@ -6793,115 +6858,115 @@
         <v/>
       </c>
       <c r="B92" s="17" t="str">
+        <v>siding</v>
+      </c>
+      <c r="C92" s="17" t="str">
+        <v>Siding</v>
+      </c>
+      <c r="D92" s="17" t="str">
+        <v>needs-scheduled</v>
+      </c>
+      <c r="E92" s="17" t="str">
+        <v/>
+      </c>
+      <c r="F92" s="17" t="str">
+        <v/>
+      </c>
+      <c r="G92" s="17" t="str">
+        <v>propane</v>
+      </c>
+      <c r="H92" s="17" t="str">
+        <v/>
+      </c>
+      <c r="I92" s="17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="9" t="str">
+        <v/>
+      </c>
+      <c r="B93" s="9" t="str">
         <v>siding-2</v>
       </c>
-      <c r="C92" s="17" t="str">
+      <c r="C93" s="9" t="str">
         <v xml:space="preserve">  ↳ Siding</v>
       </c>
-      <c r="D92" s="17" t="str">
-        <v>needs-scheduled</v>
-      </c>
-      <c r="E92" s="17" t="str">
-        <v/>
-      </c>
-      <c r="F92" s="17" t="str">
-        <v/>
-      </c>
-      <c r="G92" s="17" t="str">
-        <v/>
-      </c>
-      <c r="H92" s="17" t="str">
-        <v/>
-      </c>
-      <c r="I92" s="17" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="2" t="str">
-        <v/>
-      </c>
-      <c r="B93" s="2" t="str">
-        <v/>
-      </c>
-      <c r="C93" s="2" t="str">
-        <v/>
-      </c>
-      <c r="D93" s="2" t="str">
-        <v/>
-      </c>
-      <c r="E93" s="2" t="str">
-        <v/>
-      </c>
-      <c r="F93" s="2" t="str">
-        <v/>
-      </c>
-      <c r="G93" s="2" t="str">
-        <v/>
-      </c>
-      <c r="H93" s="2" t="str">
-        <v/>
-      </c>
-      <c r="I93" s="2" t="str">
+      <c r="D93" s="9" t="str">
+        <v>needs-scheduled</v>
+      </c>
+      <c r="E93" s="9" t="str">
+        <v/>
+      </c>
+      <c r="F93" s="9" t="str">
+        <v/>
+      </c>
+      <c r="G93" s="9" t="str">
+        <v/>
+      </c>
+      <c r="H93" s="9" t="str">
+        <v/>
+      </c>
+      <c r="I93" s="9" t="str">
         <v/>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="16" t="str">
+      <c r="A94" s="2" t="str">
+        <v/>
+      </c>
+      <c r="B94" s="2" t="str">
+        <v/>
+      </c>
+      <c r="C94" s="2" t="str">
+        <v/>
+      </c>
+      <c r="D94" s="2" t="str">
+        <v/>
+      </c>
+      <c r="E94" s="2" t="str">
+        <v/>
+      </c>
+      <c r="F94" s="2" t="str">
+        <v/>
+      </c>
+      <c r="G94" s="2" t="str">
+        <v/>
+      </c>
+      <c r="H94" s="2" t="str">
+        <v/>
+      </c>
+      <c r="I94" s="2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="16" t="str">
         <v>▶ Unassigned (14 items)</v>
       </c>
-      <c r="B94" s="16" t="str">
-        <v/>
-      </c>
-      <c r="C94" s="16" t="str">
-        <v/>
-      </c>
-      <c r="D94" s="16" t="str">
-        <v/>
-      </c>
-      <c r="E94" s="16" t="str">
-        <v/>
-      </c>
-      <c r="F94" s="16" t="str">
-        <v/>
-      </c>
-      <c r="G94" s="16" t="str">
-        <v/>
-      </c>
-      <c r="H94" s="16" t="str">
-        <v/>
-      </c>
-      <c r="I94" s="16" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="9" t="str">
-        <v/>
-      </c>
-      <c r="B95" s="9" t="str">
-        <v>crest-prep</v>
-      </c>
-      <c r="C95" s="9" t="str">
-        <v>Crest Prep / Cleaning</v>
-      </c>
-      <c r="D95" s="9" t="str">
-        <v>needs-scheduled</v>
-      </c>
-      <c r="E95" s="9" t="str">
-        <v>2026-01-26</v>
-      </c>
-      <c r="F95" s="9" t="str">
-        <v>2026-01-26</v>
-      </c>
-      <c r="G95" s="9" t="str">
-        <v>kitchen-baseboard, upper-cabinet-install, finish-trim</v>
-      </c>
-      <c r="H95" s="9" t="str">
-        <v>crest-installation</v>
-      </c>
-      <c r="I95" s="9" t="str">
-        <v>Clean and prep kitchen area before Crest arrives. Clear tools and materials, protect flooring.</v>
+      <c r="B95" s="16" t="str">
+        <v/>
+      </c>
+      <c r="C95" s="16" t="str">
+        <v/>
+      </c>
+      <c r="D95" s="16" t="str">
+        <v/>
+      </c>
+      <c r="E95" s="16" t="str">
+        <v/>
+      </c>
+      <c r="F95" s="16" t="str">
+        <v/>
+      </c>
+      <c r="G95" s="16" t="str">
+        <v/>
+      </c>
+      <c r="H95" s="16" t="str">
+        <v/>
+      </c>
+      <c r="I95" s="16" t="str">
+        <v/>
       </c>
     </row>
     <row r="96">
@@ -6909,28 +6974,28 @@
         <v/>
       </c>
       <c r="B96" s="17" t="str">
-        <v>propane</v>
+        <v>crest-prep</v>
       </c>
       <c r="C96" s="17" t="str">
-        <v>Propane</v>
+        <v>Crest Prep / Cleaning</v>
       </c>
       <c r="D96" s="17" t="str">
-        <v>scheduled</v>
+        <v>needs-scheduled</v>
       </c>
       <c r="E96" s="17" t="str">
-        <v>2026-01-23</v>
+        <v>2026-01-26</v>
       </c>
       <c r="F96" s="17" t="str">
-        <v>2026-01-23</v>
+        <v>2026-01-26</v>
       </c>
       <c r="G96" s="17" t="str">
-        <v/>
+        <v>kitchen-baseboard, upper-cabinet-install, finish-trim</v>
       </c>
       <c r="H96" s="17" t="str">
-        <v>crest-installation, install-stainless-wall, siding</v>
+        <v>crest-installation</v>
       </c>
       <c r="I96" s="17" t="str">
-        <v>Dave coordinating and responsible. Dependency for siding install.</v>
+        <v>Clean and prep kitchen area before Crest arrives. Clear tools and materials, protect flooring.</v>
       </c>
     </row>
     <row r="97">
@@ -6938,28 +7003,28 @@
         <v/>
       </c>
       <c r="B97" s="9" t="str">
-        <v>kitchen-put-back</v>
+        <v>propane</v>
       </c>
       <c r="C97" s="9" t="str">
-        <v>Kitchen Put-Back</v>
+        <v>Propane</v>
       </c>
       <c r="D97" s="9" t="str">
-        <v>needs-scheduled</v>
+        <v>scheduled</v>
       </c>
       <c r="E97" s="9" t="str">
-        <v/>
+        <v>2026-01-23</v>
       </c>
       <c r="F97" s="9" t="str">
-        <v/>
+        <v>2026-01-23</v>
       </c>
       <c r="G97" s="9" t="str">
-        <v>crest-installation, finish-plumbing</v>
+        <v/>
       </c>
       <c r="H97" s="9" t="str">
-        <v>project-finish</v>
+        <v>crest-installation, install-stainless-wall, siding</v>
       </c>
       <c r="I97" s="9" t="str">
-        <v/>
+        <v>Dave coordinating and responsible. Dependency for siding install.</v>
       </c>
     </row>
     <row r="98">
@@ -6967,10 +7032,10 @@
         <v/>
       </c>
       <c r="B98" s="17" t="str">
-        <v>kitchen-put-back-2</v>
+        <v>kitchen-put-back</v>
       </c>
       <c r="C98" s="17" t="str">
-        <v xml:space="preserve">  ↳ Install Ovens</v>
+        <v>Kitchen Put-Back</v>
       </c>
       <c r="D98" s="17" t="str">
         <v>needs-scheduled</v>
@@ -6982,10 +7047,10 @@
         <v/>
       </c>
       <c r="G98" s="17" t="str">
-        <v/>
+        <v>crest-installation, finish-plumbing</v>
       </c>
       <c r="H98" s="17" t="str">
-        <v/>
+        <v>project-finish</v>
       </c>
       <c r="I98" s="17" t="str">
         <v/>
@@ -6996,10 +7061,10 @@
         <v/>
       </c>
       <c r="B99" s="9" t="str">
-        <v>kitchen-put-back-3</v>
+        <v>kitchen-put-back-2</v>
       </c>
       <c r="C99" s="9" t="str">
-        <v xml:space="preserve">  ↳ Move Range, Freezers and Refrigerators</v>
+        <v xml:space="preserve">  ↳ Install Ovens</v>
       </c>
       <c r="D99" s="9" t="str">
         <v>needs-scheduled</v>
@@ -7025,10 +7090,10 @@
         <v/>
       </c>
       <c r="B100" s="17" t="str">
-        <v>install-dryer-vents</v>
+        <v>kitchen-put-back-3</v>
       </c>
       <c r="C100" s="17" t="str">
-        <v>Install Dryer Vents</v>
+        <v xml:space="preserve">  ↳ Move Range, Freezers and Refrigerators</v>
       </c>
       <c r="D100" s="17" t="str">
         <v>needs-scheduled</v>
@@ -7046,7 +7111,7 @@
         <v/>
       </c>
       <c r="I100" s="17" t="str">
-        <v>Cut holes from laundry room to outside for dryer vents.</v>
+        <v/>
       </c>
     </row>
     <row r="101">
@@ -7054,10 +7119,10 @@
         <v/>
       </c>
       <c r="B101" s="9" t="str">
-        <v>misc-equipment-install</v>
+        <v>install-dryer-vents</v>
       </c>
       <c r="C101" s="9" t="str">
-        <v>Misc Equipment Install</v>
+        <v>Install Dryer Vents</v>
       </c>
       <c r="D101" s="9" t="str">
         <v>needs-scheduled</v>
@@ -7075,7 +7140,7 @@
         <v/>
       </c>
       <c r="I101" s="9" t="str">
-        <v/>
+        <v>Cut holes from laundry room to outside for dryer vents.</v>
       </c>
     </row>
     <row r="102">
@@ -7083,10 +7148,10 @@
         <v/>
       </c>
       <c r="B102" s="17" t="str">
-        <v>misc-equipment-install-1</v>
+        <v>misc-equipment-install</v>
       </c>
       <c r="C102" s="17" t="str">
-        <v xml:space="preserve">  ↳ Install Pot Rack</v>
+        <v>Misc Equipment Install</v>
       </c>
       <c r="D102" s="17" t="str">
         <v>needs-scheduled</v>
@@ -7112,10 +7177,10 @@
         <v/>
       </c>
       <c r="B103" s="9" t="str">
-        <v>misc-equipment-install-2</v>
+        <v>misc-equipment-install-1</v>
       </c>
       <c r="C103" s="9" t="str">
-        <v xml:space="preserve">  ↳ Install Retractable Extension Cord</v>
+        <v xml:space="preserve">  ↳ Install Pot Rack</v>
       </c>
       <c r="D103" s="9" t="str">
         <v>needs-scheduled</v>
@@ -7141,28 +7206,28 @@
         <v/>
       </c>
       <c r="B104" s="17" t="str">
-        <v>upper-cabinet-install</v>
+        <v>misc-equipment-install-2</v>
       </c>
       <c r="C104" s="17" t="str">
-        <v>Upper Cabinet Install</v>
+        <v xml:space="preserve">  ↳ Install Retractable Extension Cord</v>
       </c>
       <c r="D104" s="17" t="str">
-        <v>scheduled</v>
+        <v>needs-scheduled</v>
       </c>
       <c r="E104" s="17" t="str">
-        <v>2026-01-26</v>
+        <v/>
       </c>
       <c r="F104" s="17" t="str">
-        <v>2026-01-26</v>
+        <v/>
       </c>
       <c r="G104" s="17" t="str">
-        <v>finish-trim</v>
+        <v/>
       </c>
       <c r="H104" s="17" t="str">
-        <v>crest-prep, crest-installation</v>
+        <v/>
       </c>
       <c r="I104" s="17" t="str">
-        <v>Requires cabinet crown installation.</v>
+        <v/>
       </c>
     </row>
     <row r="105">
@@ -7170,28 +7235,28 @@
         <v/>
       </c>
       <c r="B105" s="9" t="str">
-        <v>upper-cabinet-install-1</v>
+        <v>upper-cabinet-install</v>
       </c>
       <c r="C105" s="9" t="str">
-        <v xml:space="preserve">  ↳ Upper Cabinet Delivery</v>
+        <v>Upper Cabinet Install</v>
       </c>
       <c r="D105" s="9" t="str">
-        <v>confirmed</v>
+        <v>scheduled</v>
       </c>
       <c r="E105" s="9" t="str">
-        <v>2026-01-22</v>
+        <v>2026-01-26</v>
       </c>
       <c r="F105" s="9" t="str">
-        <v>2026-01-22</v>
+        <v>2026-01-26</v>
       </c>
       <c r="G105" s="9" t="str">
-        <v/>
+        <v>finish-trim</v>
       </c>
       <c r="H105" s="9" t="str">
-        <v/>
+        <v>crest-prep, crest-installation</v>
       </c>
       <c r="I105" s="9" t="str">
-        <v/>
+        <v>Requires cabinet crown installation.</v>
       </c>
     </row>
     <row r="106">
@@ -7199,19 +7264,19 @@
         <v/>
       </c>
       <c r="B106" s="17" t="str">
-        <v>upper-cabinet-install-3</v>
+        <v>upper-cabinet-install-1</v>
       </c>
       <c r="C106" s="17" t="str">
-        <v xml:space="preserve">  ↳ Install Upper Cabinets</v>
+        <v xml:space="preserve">  ↳ Upper Cabinet Delivery</v>
       </c>
       <c r="D106" s="17" t="str">
-        <v>needs-scheduled</v>
+        <v>confirmed</v>
       </c>
       <c r="E106" s="17" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-22</v>
       </c>
       <c r="F106" s="17" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-22</v>
       </c>
       <c r="G106" s="17" t="str">
         <v/>
@@ -7228,28 +7293,28 @@
         <v/>
       </c>
       <c r="B107" s="9" t="str">
-        <v>project-finish</v>
+        <v>upper-cabinet-install-3</v>
       </c>
       <c r="C107" s="9" t="str">
-        <v>Project Finish</v>
+        <v xml:space="preserve">  ↳ Install Upper Cabinets</v>
       </c>
       <c r="D107" s="9" t="str">
         <v>needs-scheduled</v>
       </c>
       <c r="E107" s="9" t="str">
-        <v/>
+        <v>2026-01-26</v>
       </c>
       <c r="F107" s="9" t="str">
-        <v/>
+        <v>2026-01-26</v>
       </c>
       <c r="G107" s="9" t="str">
-        <v>inspection, crest-installation, kitchen-put-back, close-permit</v>
+        <v/>
       </c>
       <c r="H107" s="9" t="str">
         <v/>
       </c>
       <c r="I107" s="9" t="str">
-        <v>Final punch acceptance criteria: All work complete per contract scope, all inspections passed, all equipment operational, no safety hazards, cosmetic defects documented and remediated.</v>
+        <v/>
       </c>
     </row>
     <row r="108">
@@ -7257,71 +7322,100 @@
         <v/>
       </c>
       <c r="B108" s="17" t="str">
+        <v>project-finish</v>
+      </c>
+      <c r="C108" s="17" t="str">
+        <v>Project Finish</v>
+      </c>
+      <c r="D108" s="17" t="str">
+        <v>needs-scheduled</v>
+      </c>
+      <c r="E108" s="17" t="str">
+        <v/>
+      </c>
+      <c r="F108" s="17" t="str">
+        <v/>
+      </c>
+      <c r="G108" s="17" t="str">
+        <v>inspection, crest-installation, kitchen-put-back, close-permit</v>
+      </c>
+      <c r="H108" s="17" t="str">
+        <v/>
+      </c>
+      <c r="I108" s="17" t="str">
+        <v>Final punch acceptance criteria: All work complete per contract scope, all inspections passed, all equipment operational, no safety hazards, cosmetic defects documented and remediated.</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="9" t="str">
+        <v/>
+      </c>
+      <c r="B109" s="9" t="str">
         <v>install-hvac-registers</v>
       </c>
-      <c r="C108" s="17" t="str">
+      <c r="C109" s="9" t="str">
         <v>Install HVAC Registers</v>
       </c>
-      <c r="D108" s="17" t="str">
-        <v>needs-scheduled</v>
-      </c>
-      <c r="E108" s="17" t="str">
-        <v/>
-      </c>
-      <c r="F108" s="17" t="str">
-        <v/>
-      </c>
-      <c r="G108" s="17" t="str">
-        <v/>
-      </c>
-      <c r="H108" s="17" t="str">
-        <v/>
-      </c>
-      <c r="I108" s="17" t="str">
+      <c r="D109" s="9" t="str">
+        <v>needs-scheduled</v>
+      </c>
+      <c r="E109" s="9" t="str">
+        <v/>
+      </c>
+      <c r="F109" s="9" t="str">
+        <v/>
+      </c>
+      <c r="G109" s="9" t="str">
+        <v/>
+      </c>
+      <c r="H109" s="9" t="str">
+        <v/>
+      </c>
+      <c r="I109" s="9" t="str">
         <v>Need to check with Chad if he's providing and installing these</v>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" s="2" t="str">
-        <v/>
-      </c>
-      <c r="B109" s="2" t="str">
-        <v/>
-      </c>
-      <c r="C109" s="2" t="str">
-        <v/>
-      </c>
-      <c r="D109" s="2" t="str">
-        <v/>
-      </c>
-      <c r="E109" s="2" t="str">
-        <v/>
-      </c>
-      <c r="F109" s="2" t="str">
-        <v/>
-      </c>
-      <c r="G109" s="2" t="str">
-        <v/>
-      </c>
-      <c r="H109" s="2" t="str">
-        <v/>
-      </c>
-      <c r="I109" s="2" t="str">
+    <row r="110">
+      <c r="A110" s="2" t="str">
+        <v/>
+      </c>
+      <c r="B110" s="2" t="str">
+        <v/>
+      </c>
+      <c r="C110" s="2" t="str">
+        <v/>
+      </c>
+      <c r="D110" s="2" t="str">
+        <v/>
+      </c>
+      <c r="E110" s="2" t="str">
+        <v/>
+      </c>
+      <c r="F110" s="2" t="str">
+        <v/>
+      </c>
+      <c r="G110" s="2" t="str">
+        <v/>
+      </c>
+      <c r="H110" s="2" t="str">
+        <v/>
+      </c>
+      <c r="I110" s="2" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <autoFilter ref="A1:I109"/>
+  <autoFilter ref="A1:I110"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I109"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I110"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N81"/>
+  <dimension ref="A1:N82"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10914,18 +11008,62 @@
         <v/>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" s="7" t="str">
+        <v>TASK</v>
+      </c>
+      <c r="B82" s="7" t="str">
+        <v>hvac-finish</v>
+      </c>
+      <c r="C82" s="7" t="str">
+        <v>Schedule HVAC Finish</v>
+      </c>
+      <c r="D82" s="7" t="str">
+        <v>needs-scheduled</v>
+      </c>
+      <c r="E82" s="7" t="str">
+        <v>⚠️ Missing: dates</v>
+      </c>
+      <c r="F82" s="7" t="str">
+        <v/>
+      </c>
+      <c r="G82" s="7" t="str">
+        <v/>
+      </c>
+      <c r="H82" s="7" t="str">
+        <v>Joclar &amp; Fields</v>
+      </c>
+      <c r="I82" s="7" t="str">
+        <v>mechanical</v>
+      </c>
+      <c r="J82" s="7" t="str">
+        <v/>
+      </c>
+      <c r="K82" s="7" t="str">
+        <v/>
+      </c>
+      <c r="L82" s="7" t="str">
+        <v>hvac-registers, hvac-cold-air-return</v>
+      </c>
+      <c r="M82" s="7" t="str">
+        <v/>
+      </c>
+      <c r="N82" s="2" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <autoFilter ref="A1:M81"/>
+  <autoFilter ref="A1:M82"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N81"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N82"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11552,11 +11690,87 @@
         <v/>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" s="9" t="str">
+        <v>hvac-registers</v>
+      </c>
+      <c r="B17" s="9" t="str">
+        <v>HVAC Registers</v>
+      </c>
+      <c r="C17" s="9" t="str">
+        <v>vendor-provided</v>
+      </c>
+      <c r="D17" s="9" t="str">
+        <v>✅ Yes</v>
+      </c>
+      <c r="E17" s="9" t="str">
+        <v>hvac-finish</v>
+      </c>
+      <c r="F17" s="9" t="str">
+        <v/>
+      </c>
+      <c r="G17" s="9">
+        <v>8</v>
+      </c>
+      <c r="H17" s="9" t="str">
+        <v/>
+      </c>
+      <c r="I17" s="9" t="str">
+        <v/>
+      </c>
+      <c r="J17" s="9" t="str">
+        <v>White</v>
+      </c>
+      <c r="K17" s="9" t="str">
+        <v/>
+      </c>
+      <c r="L17" s="9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="17" t="str">
+        <v>hvac-cold-air-return</v>
+      </c>
+      <c r="B18" s="17" t="str">
+        <v>HVAC Cold Air Return Cover</v>
+      </c>
+      <c r="C18" s="17" t="str">
+        <v>vendor-provided</v>
+      </c>
+      <c r="D18" s="17" t="str">
+        <v>✅ Yes</v>
+      </c>
+      <c r="E18" s="17" t="str">
+        <v>hvac-finish</v>
+      </c>
+      <c r="F18" s="17" t="str">
+        <v/>
+      </c>
+      <c r="G18" s="17">
+        <v>1</v>
+      </c>
+      <c r="H18" s="17" t="str">
+        <v/>
+      </c>
+      <c r="I18" s="17" t="str">
+        <v/>
+      </c>
+      <c r="J18" s="17" t="str">
+        <v>White</v>
+      </c>
+      <c r="K18" s="17" t="str">
+        <v/>
+      </c>
+      <c r="L18" s="17" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <autoFilter ref="A1:L16"/>
+  <autoFilter ref="A1:L18"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L18"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>